<commit_message>
feat: Added logging and error handling, refactored code
The following changes have been made:
- Logging added to improve program traceability.
- Code refactoring conducted to enhance readability and maintainability.
- Error handling, including trigger-related errors, has been implemented.
</commit_message>
<xml_diff>
--- a/src/main/resources/reportGoods.xlsx
+++ b/src/main/resources/reportGoods.xlsx
@@ -13,15 +13,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Name</t>
   </si>
   <si>
     <t>Priority</t>
-  </si>
-  <si>
-    <t>крупа</t>
   </si>
   <si>
     <t>лук</t>
@@ -34,12 +31,6 @@
   </si>
   <si>
     <t>лапша</t>
-  </si>
-  <si>
-    <t>чича</t>
-  </si>
-  <si>
-    <t>fertgreg</t>
   </si>
 </sst>
 </file>
@@ -109,7 +100,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -117,7 +108,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -125,7 +116,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -133,31 +124,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="n">
         <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="n">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>